<commit_message>
835 Medium Bit OP Class:?
</commit_message>
<xml_diff>
--- a/Trace.xlsx
+++ b/Trace.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11013"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7A374CD-D1F8-D140-8C1A-287E284E2888}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1778282A-FEE3-DF40-A30F-890FA0F83C3F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="10140" yWindow="1980" windowWidth="22260" windowHeight="12640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="72">
   <si>
     <t>Legend</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -310,6 +310,14 @@
   </si>
   <si>
     <t>Random Point in Non-overlapping Rectangles</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve"> Image Overlap</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TIME EXCEED</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -674,10 +682,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L25"/>
+  <dimension ref="A1:L26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="K29" sqref="K29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="18"/>
@@ -1249,7 +1257,7 @@
         <v>0.72916666666666663</v>
       </c>
       <c r="I17" s="3">
-        <f t="shared" ref="I17:I25" si="1">H17-G17</f>
+        <f t="shared" ref="I17:I26" si="1">H17-G17</f>
         <v>5.4861111111111027E-2</v>
       </c>
       <c r="J17" s="5">
@@ -1515,6 +1523,36 @@
       </c>
       <c r="K25" s="5">
         <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11">
+      <c r="A26" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="C26" s="1">
+        <v>835</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="G26" s="3">
+        <v>0.86111111111111116</v>
+      </c>
+      <c r="H26" s="3">
+        <v>0.95833333333333337</v>
+      </c>
+      <c r="I26" s="3">
+        <f t="shared" si="1"/>
+        <v>9.722222222222221E-2</v>
+      </c>
+      <c r="J26" s="5" t="s">
+        <v>71</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
199 py and cpp
</commit_message>
<xml_diff>
--- a/Trace.xlsx
+++ b/Trace.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11110"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BD58C2E-88AF-374F-82D8-E0CC2FB1F7EA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7CBE0D3-9BAF-ED40-9CBE-D1C8D69867E9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10140" yWindow="1980" windowWidth="22260" windowHeight="12640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10140" yWindow="1980" windowWidth="22260" windowHeight="12640" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Python" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="80">
   <si>
     <t>Legend</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -343,6 +343,14 @@
   </si>
   <si>
     <t>Goudy</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Binary Tree Right Side View</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MEdium</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -707,10 +715,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L29"/>
+  <dimension ref="A1:L30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection sqref="A1:L1"/>
+    <sheetView topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="A30" sqref="A30:F30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="18"/>
@@ -1282,7 +1290,7 @@
         <v>0.72916666666666663</v>
       </c>
       <c r="I17" s="3">
-        <f t="shared" ref="I17:I29" si="1">H17-G17</f>
+        <f t="shared" ref="I17:I30" si="1">H17-G17</f>
         <v>5.4861111111111027E-2</v>
       </c>
       <c r="J17" s="5">
@@ -1676,6 +1684,42 @@
         <v>0.98</v>
       </c>
       <c r="K29" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11">
+      <c r="A30" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B30" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="C30" s="1">
+        <v>199</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G30" s="3">
+        <v>0.85416666666666663</v>
+      </c>
+      <c r="H30" s="3">
+        <v>0.9375</v>
+      </c>
+      <c r="I30" s="1">
+        <f t="shared" si="1"/>
+        <v>8.333333333333337E-2</v>
+      </c>
+      <c r="J30" s="5">
+        <v>0.95</v>
+      </c>
+      <c r="K30" s="5">
         <v>1</v>
       </c>
     </row>
@@ -1688,13 +1732,22 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F29D91D-730D-3643-9A08-68E05AF8E7C2}">
-  <dimension ref="A1:L1"/>
+  <dimension ref="A1:L2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="7.5" customWidth="1"/>
+    <col min="2" max="2" width="27.6640625" customWidth="1"/>
+    <col min="3" max="4" width="8.83203125"/>
+    <col min="5" max="5" width="12.6640625" customWidth="1"/>
+    <col min="6" max="6" width="11" customWidth="1"/>
+    <col min="9" max="9" width="18" style="3" customWidth="1"/>
+    <col min="11" max="11" width="13.6640625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:12">
       <c r="A1" s="2" t="s">
@@ -1721,7 +1774,7 @@
       <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="I1" s="3" t="s">
         <v>8</v>
       </c>
       <c r="J1" s="2" t="s">
@@ -1733,6 +1786,43 @@
       <c r="L1" s="2" t="s">
         <v>39</v>
       </c>
+    </row>
+    <row r="2" spans="1:12" ht="17">
+      <c r="A2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="C2" s="1">
+        <v>199</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2" s="3">
+        <v>0.85416666666666663</v>
+      </c>
+      <c r="H2" s="6">
+        <v>1.0013888888888889</v>
+      </c>
+      <c r="I2" s="3">
+        <f>H2-G2</f>
+        <v>0.14722222222222225</v>
+      </c>
+      <c r="J2" s="1">
+        <v>72</v>
+      </c>
+      <c r="K2" s="1">
+        <v>100</v>
+      </c>
+      <c r="L2" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>

<commit_message>
1175 20 241 python
</commit_message>
<xml_diff>
--- a/Trace.xlsx
+++ b/Trace.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11208"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{051D81A8-8096-2F44-8345-52B0D84CBD56}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87126A16-888A-5944-89A2-500918E2EB44}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="10140" yWindow="1980" windowWidth="22260" windowHeight="12640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="88">
   <si>
     <t>Legend</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -373,6 +373,18 @@
   </si>
   <si>
     <t>Decrease Elements To Make Array Zigzag</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Different Ways to Add Parentheses</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve"> Prime Arrangements</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Valid Parentheses</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -737,10 +749,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L33"/>
+  <dimension ref="A1:L36"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
-      <selection activeCell="F38" sqref="F38"/>
+      <selection activeCell="G36" sqref="G36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="18"/>
@@ -1801,7 +1813,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="34">
+    <row r="33" spans="1:4" ht="34">
       <c r="A33" s="1" t="s">
         <v>17</v>
       </c>
@@ -1810,6 +1822,51 @@
       </c>
       <c r="C33" s="1">
         <v>1144</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4">
+      <c r="A34" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B34" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="C34" s="1">
+        <v>241</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4">
+      <c r="A35" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B35" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="C35" s="1">
+        <v>1175</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4">
+      <c r="A36" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B36" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="C36" s="1">
+        <v>20</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
1010 Y 542 Y py
</commit_message>
<xml_diff>
--- a/Trace.xlsx
+++ b/Trace.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10113"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D10D1691-D477-2E4F-A285-95A6737051AC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{981A742F-064F-3842-B9B3-F18D88DF0EAC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="10120" yWindow="1960" windowWidth="22260" windowHeight="12640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="91">
   <si>
     <t>Legend</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -389,6 +389,14 @@
   </si>
   <si>
     <t>Longest Predecessor</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Find First and Last Position of Element in Sorted Array</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve"> Sort Array By Parity II</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -753,10 +761,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L37"/>
+  <dimension ref="A1:L39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
-      <selection activeCell="D39" sqref="D39"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="D45" sqref="D45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="18"/>
@@ -1885,6 +1893,28 @@
       </c>
       <c r="D37" s="1" t="s">
         <v>9</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" ht="34">
+      <c r="A38" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B38" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="C38" s="1">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4">
+      <c r="A39" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B39" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="C39" s="1">
+        <v>922</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
1010 542 01 cpp
</commit_message>
<xml_diff>
--- a/Trace.xlsx
+++ b/Trace.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10113"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{981A742F-064F-3842-B9B3-F18D88DF0EAC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E014550-2DC1-CB49-80CD-F30D1866BCED}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="10120" yWindow="1960" windowWidth="22260" windowHeight="12640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="94">
   <si>
     <t>Legend</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -397,6 +397,18 @@
   </si>
   <si>
     <t xml:space="preserve"> Sort Array By Parity II</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>01 Matrix</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Pairs of Songs With Total Durations Divisible by 60  </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Two Sum</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -761,10 +773,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L39"/>
+  <dimension ref="A1:L42"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="D45" sqref="D45"/>
+      <selection activeCell="C41" sqref="C40:C41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="18"/>
@@ -1915,6 +1927,39 @@
       </c>
       <c r="C39" s="1">
         <v>922</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" ht="34">
+      <c r="A40" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B40" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="C40" s="1">
+        <v>1010</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4">
+      <c r="A41" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B41" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="C41" s="1">
+        <v>542</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4">
+      <c r="A42" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B42" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="C42" s="1">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
1014 * py;121 Y py
</commit_message>
<xml_diff>
--- a/Trace.xlsx
+++ b/Trace.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10113"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C39AE6D-0916-F949-B607-D89E715D94A4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86AF2C22-D83A-384E-B2B8-7700795D2AA8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="10120" yWindow="1960" windowWidth="22260" windowHeight="12640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="106">
   <si>
     <t>Legend</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -445,6 +445,18 @@
   </si>
   <si>
     <t>Sum of Mutated Array Closest to Target</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Best Sightseeing Pair</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>05/02/2020</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Best Time to Buy and Sell Stock</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -818,10 +830,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L48"/>
+  <dimension ref="A1:L50"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
-      <selection activeCell="L48" sqref="L48"/>
+      <selection activeCell="M50" sqref="M50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="18"/>
@@ -2074,6 +2086,9 @@
       </c>
     </row>
     <row r="48" spans="1:12" ht="34">
+      <c r="A48" s="1" t="s">
+        <v>17</v>
+      </c>
       <c r="B48" s="4" t="s">
         <v>102</v>
       </c>
@@ -2082,6 +2097,34 @@
       </c>
       <c r="L48" s="8" t="s">
         <v>101</v>
+      </c>
+    </row>
+    <row r="49" spans="1:12">
+      <c r="A49" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B49" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="C49" s="1">
+        <v>1014</v>
+      </c>
+      <c r="L49" s="8" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="50" spans="1:12">
+      <c r="A50" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B50" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="C50" s="1">
+        <v>121</v>
+      </c>
+      <c r="L50" s="8" t="s">
+        <v>104</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
583 ? PY; 410 * PY
</commit_message>
<xml_diff>
--- a/Trace.xlsx
+++ b/Trace.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10113"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB91D3C2-FA5B-1B4D-B34D-2BBF5D18AF10}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E516D621-8D58-CC4D-85AE-50DB609CADA7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="10120" yWindow="1960" windowWidth="22260" windowHeight="12640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="112">
   <si>
     <t>Legend</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -473,6 +473,14 @@
   </si>
   <si>
     <t>Longest Substring Without Repeating Characters</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Delete Operation for Two Strings</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>11/02/2020</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -849,10 +857,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L53"/>
+  <dimension ref="A1:L54"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="L54" sqref="L54"/>
+      <selection activeCell="C55" sqref="C55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="18"/>
@@ -2180,6 +2188,20 @@
       </c>
       <c r="L53" s="9" t="s">
         <v>108</v>
+      </c>
+    </row>
+    <row r="54" spans="1:12">
+      <c r="A54" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B54" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="C54" s="1">
+        <v>583</v>
+      </c>
+      <c r="L54" s="1" t="s">
+        <v>111</v>
       </c>
     </row>
   </sheetData>

</xml_diff>